<commit_message>
Change-Id: I0000000000000000000000000000000000000000 test data updated
Change-Id: I4d3a90805c6483942f8b9b5baa5f4731a88e69c5
</commit_message>
<xml_diff>
--- a/BITSAUTOMATION/excel/TestData.xlsx
+++ b/BITSAUTOMATION/excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" tabRatio="924" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -15,19 +15,21 @@
     <sheet name="MSCourse" sheetId="8" r:id="rId6"/>
     <sheet name="MSData" sheetId="9" r:id="rId7"/>
     <sheet name="SStationList" sheetId="10" r:id="rId8"/>
-    <sheet name="SStationDetail" sheetId="11" r:id="rId9"/>
-    <sheet name="SAllotList" sheetId="12" r:id="rId10"/>
-    <sheet name="PBankList1" sheetId="13" r:id="rId11"/>
-    <sheet name="AddProblem" sheetId="14" r:id="rId12"/>
-    <sheet name="SSAllot" sheetId="15" r:id="rId13"/>
-    <sheet name="AllAllotStudentList" sheetId="16" r:id="rId14"/>
-    <sheet name="PersonalInfo" sheetId="17" r:id="rId15"/>
-    <sheet name="AddAcademic" sheetId="18" r:id="rId16"/>
-    <sheet name="ViewCourse" sheetId="19" r:id="rId17"/>
-    <sheet name="ManageStation" sheetId="3" r:id="rId18"/>
-    <sheet name="PBankList" sheetId="4" r:id="rId19"/>
+    <sheet name="Dashboard" sheetId="21" r:id="rId9"/>
+    <sheet name="SStationDetail" sheetId="11" r:id="rId10"/>
+    <sheet name="SAllotList" sheetId="12" r:id="rId11"/>
+    <sheet name="PBankList1" sheetId="13" r:id="rId12"/>
+    <sheet name="AddProblem" sheetId="14" r:id="rId13"/>
+    <sheet name="SSAllot" sheetId="15" r:id="rId14"/>
+    <sheet name="AllAllotStudentList" sheetId="16" r:id="rId15"/>
+    <sheet name="PersonalInfo" sheetId="17" r:id="rId16"/>
+    <sheet name="AddAcademic" sheetId="18" r:id="rId17"/>
+    <sheet name="ViewCourse" sheetId="19" r:id="rId18"/>
+    <sheet name="ManageStation" sheetId="3" r:id="rId19"/>
+    <sheet name="PBankList" sheetId="4" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="376">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>rajeevmkartha@gmail.com</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -54,16 +53,7 @@
     <t>role</t>
   </si>
   <si>
-    <t>student</t>
-  </si>
-  <si>
-    <t>faculty</t>
-  </si>
-  <si>
     <t>rajeevmkartha@outlook.com</t>
-  </si>
-  <si>
-    <t>Raj M Kartha</t>
   </si>
   <si>
     <t>Female</t>
@@ -253,12 +243,6 @@
     <t>Faculty Name</t>
   </si>
   <si>
-    <t>Kalasree Yahoo</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
     <t>Goa</t>
   </si>
   <si>
@@ -301,21 +285,12 @@
     <t>PIN</t>
   </si>
   <si>
-    <t>Lokesh Gmail</t>
-  </si>
-  <si>
-    <t>PSRN000020</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>Mathematics</t>
   </si>
   <si>
-    <t>Test15@yahoo.com</t>
-  </si>
-  <si>
     <t>9999999999</t>
   </si>
   <si>
@@ -358,12 +333,6 @@
     <t>PO EDATHALA, Kolkata</t>
   </si>
   <si>
-    <t>UAE</t>
-  </si>
-  <si>
-    <t>Dubai</t>
-  </si>
-  <si>
     <t>Phoenix</t>
   </si>
   <si>
@@ -376,9 +345,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>Test Student 1</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -400,9 +366,6 @@
     <t>Campus ID</t>
   </si>
   <si>
-    <t>2015B4A30621H</t>
-  </si>
-  <si>
     <t>Campus Name</t>
   </si>
   <si>
@@ -415,9 +378,6 @@
     <t>BITS Goa</t>
   </si>
   <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
     <t>BITS India Ltd</t>
   </si>
   <si>
@@ -931,12 +891,6 @@
     <t>Software Skills</t>
   </si>
   <si>
-    <t>somelogin@login.com</t>
-  </si>
-  <si>
-    <t>Invalidid</t>
-  </si>
-  <si>
     <t>Scenarios to check</t>
   </si>
   <si>
@@ -1025,13 +979,202 @@
   </si>
   <si>
     <t>when problems bank specifies 10 students irrespective of gender, the 10 most eligible students should only be selected based on cgpa, discipline etc irrespective of gender</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>sandeep_g@preludesys.com</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>varun.dewal@pilani.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>Allotment</t>
+  </si>
+  <si>
+    <t>allotment@bits.com</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Varun.singh@pilani.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>dean@bits.com</t>
+  </si>
+  <si>
+    <t>instruction_cell@bits.com</t>
+  </si>
+  <si>
+    <t>invalidid@bits.com</t>
+  </si>
+  <si>
+    <t>Invalid Id</t>
+  </si>
+  <si>
+    <t>RKartha1</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Test Upload Faculty</t>
+  </si>
+  <si>
+    <t>TKartha7</t>
+  </si>
+  <si>
+    <t>AreaSpclzn</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Rokesh Gmail6</t>
+  </si>
+  <si>
+    <t>PSRNT00006</t>
+  </si>
+  <si>
+    <t>PSRNT00006@bits.com</t>
+  </si>
+  <si>
+    <t>BHUVAN SHARMA .</t>
+  </si>
+  <si>
+    <t>2019B1A10986P</t>
+  </si>
+  <si>
+    <t>A - Student test1</t>
+  </si>
+  <si>
+    <t>Test Student38</t>
+  </si>
+  <si>
+    <t>Kulkarni</t>
+  </si>
+  <si>
+    <t>Test My Course Upload</t>
+  </si>
+  <si>
+    <t>Invalid Station</t>
+  </si>
+  <si>
+    <t>Wipro Chennai</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Statuses</t>
+  </si>
+  <si>
+    <t>Consent received</t>
+  </si>
+  <si>
+    <t>PS Types</t>
+  </si>
+  <si>
+    <t>Page Header</t>
+  </si>
+  <si>
+    <t>Practice School</t>
+  </si>
+  <si>
+    <t>Current Batch</t>
+  </si>
+  <si>
+    <t>Station Allotment Details</t>
+  </si>
+  <si>
+    <t>Allotted</t>
+  </si>
+  <si>
+    <t>Allotted to Non-core Discipline</t>
+  </si>
+  <si>
+    <t>Total Students</t>
+  </si>
+  <si>
+    <t>Allotted Students</t>
+  </si>
+  <si>
+    <t>Allotted Organizations</t>
+  </si>
+  <si>
+    <t>Organizations Announced</t>
+  </si>
+  <si>
+    <t>Allotted to Core Discipline</t>
+  </si>
+  <si>
+    <t>Allotted Within Top 5 Preferences</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Stations Participated</t>
+  </si>
+  <si>
+    <t>Station Allotted</t>
+  </si>
+  <si>
+    <t>Total Allotted</t>
+  </si>
+  <si>
+    <t>Total Requirements</t>
+  </si>
+  <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Lowest</t>
+  </si>
+  <si>
+    <t>Practice School - PS II</t>
+  </si>
+  <si>
+    <t>Current Batch - 2021-22</t>
+  </si>
+  <si>
+    <t>Semester - Semester 1</t>
+  </si>
+  <si>
+    <t>Station Announced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1046,6 +1189,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1074,7 +1223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1092,19 +1241,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1146,7 +1282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1160,31 +1296,43 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1469,7 +1617,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1488,55 +1636,53 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>123456</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>313</v>
+      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3" s="3" t="s">
+        <v>316</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D4" s="1"/>
+      <c r="A4" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1547,10 +1693,14 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1561,10 +1711,16 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1575,10 +1731,16 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1589,10 +1751,16 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1603,10 +1771,16 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1674,91 +1848,181 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="B2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>164</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>171</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="P3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,6 +2030,88 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -1782,17 +2128,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1801,7 +2147,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1812,66 +2158,66 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>49</v>
+      <c r="A5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1911,7 +2257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
@@ -1922,429 +2268,429 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="A1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>182</v>
+      <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E4" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="A5" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>200</v>
+      <c r="A6" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="A9" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="I10" s="12"/>
+      <c r="A10" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
-        <v>220</v>
+      <c r="B12" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="10" t="s">
-        <v>221</v>
+      <c r="D12" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="A13" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>224</v>
+      <c r="A14" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>227</v>
+      <c r="A16" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="A17" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>140</v>
+      <c r="A18" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="I20" s="4" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -2375,25 +2721,25 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2401,54 +2747,54 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
-        <v>260</v>
+      <c r="B5" s="9" t="s">
+        <v>246</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E6" s="4" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E7" s="11" t="s">
-        <v>262</v>
+      <c r="E7" s="10" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2456,7 +2802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -2468,22 +2814,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2491,7 +2837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -2514,53 +2860,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="A1" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>271</v>
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -2568,83 +2914,83 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="A5" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>86</v>
+      <c r="A6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2659,7 +3005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2678,83 +3024,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>285</v>
+      <c r="A1" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>296</v>
+      <c r="A4" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2762,7 +3108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2774,34 +3120,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2809,7 +3155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2828,92 +3174,92 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2922,7 +3268,169 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2938,212 +3446,63 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="C1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="20" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>306</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="20" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B12" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>325</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3153,10 +3512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3166,106 +3525,127 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="13.08984375" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" customWidth="1"/>
+    <col min="14" max="14" width="5.90625" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="N1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="21">
+        <v>1234567890</v>
+      </c>
+      <c r="H2" s="21">
+        <v>1234741258</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="21">
+        <v>55555</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:15" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>1234567890</v>
-      </c>
-      <c r="H2">
-        <v>1234741258</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2">
-        <v>55555</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3281,257 +3661,290 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>328</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>329</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection sqref="A1:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="6" t="s">
+      <c r="K2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3542,71 +3955,87 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://psmswebqastore.z30.web.core.windows.net/faculty/edit/683"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>343</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>117</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3615,83 +4044,99 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3704,16 +4149,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3724,7 +4169,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>123</v>
+        <v>345</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3736,16 +4181,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>346</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3755,19 +4200,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3776,19 +4221,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>126</v>
+        <v>37</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>347</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -3798,16 +4243,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -3817,16 +4262,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3845,12 +4290,12 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3859,16 +4304,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -3879,7 +4324,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3891,16 +4336,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3910,19 +4355,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -3931,19 +4376,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -3953,16 +4398,16 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -3971,196 +4416,283 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>156</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="P3" s="1"/>
+      <c r="B3" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>364</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>375</v>
+      </c>
+      <c r="B13" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>367</v>
+      </c>
+      <c r="B15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17">
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>369</v>
+      </c>
+      <c r="B18">
+        <v>100650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>371</v>
+      </c>
+      <c r="B20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>355</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change-Id: I0000000000000000000000000000000000000000 Commit all
Change-Id: I41cb4a6df27a3e159d2ebb6a786170d5a67d6e35
</commit_message>
<xml_diff>
--- a/BITSAUTOMATION/excel/TestData.xlsx
+++ b/BITSAUTOMATION/excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" tabRatio="924" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" tabRatio="924" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="PBankList" sheetId="4" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="389">
   <si>
     <t>username</t>
   </si>
@@ -53,9 +52,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>rajeevmkartha@outlook.com</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -140,9 +136,6 @@
     <t>Off Campus</t>
   </si>
   <si>
-    <t>Biological Science</t>
-  </si>
-  <si>
     <t>TestStation</t>
   </si>
   <si>
@@ -162,9 +155,6 @@
   </si>
   <si>
     <t>Created By</t>
-  </si>
-  <si>
-    <t>UIIL</t>
   </si>
   <si>
     <t>PS I</t>
@@ -186,9 +176,6 @@
     <t>Insurance</t>
   </si>
   <si>
-    <t>lnt</t>
-  </si>
-  <si>
     <t>In Process</t>
   </si>
   <si>
@@ -213,9 +200,6 @@
     <t>Search By</t>
   </si>
   <si>
-    <t>ncr</t>
-  </si>
-  <si>
     <t>Station City</t>
   </si>
   <si>
@@ -1168,6 +1152,60 @@
   </si>
   <si>
     <t>Station Announced</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Average station Allotted</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Varun.singhpilani.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>1234A</t>
+  </si>
+  <si>
+    <t>12345A</t>
+  </si>
+  <si>
+    <t>a12345678</t>
+  </si>
+  <si>
+    <t>a1234567890</t>
+  </si>
+  <si>
+    <t>Suzlon Energy Limited</t>
+  </si>
+  <si>
+    <t>Afour</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>testdelete</t>
+  </si>
+  <si>
+    <t>Latest</t>
+  </si>
+  <si>
+    <t>Latest3</t>
+  </si>
+  <si>
+    <t>Viram Technologies</t>
+  </si>
+  <si>
+    <t>2021-21</t>
+  </si>
+  <si>
+    <t>2022-23</t>
+  </si>
+  <si>
+    <t>2023-24</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1277,12 +1315,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1307,18 +1354,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1333,6 +1368,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1617,7 +1675,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1642,45 +1700,45 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>314</v>
+      <c r="A2" s="16" t="s">
+        <v>309</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
@@ -1698,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
@@ -1712,13 +1770,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
@@ -1732,13 +1790,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
@@ -1752,13 +1810,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
@@ -1772,13 +1830,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
@@ -1860,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1882,150 +1940,303 @@
     <col min="15" max="15" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="K3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2021</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2021</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6" t="s">
+        <v>373</v>
+      </c>
+      <c r="L6">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>13</v>
+      </c>
+      <c r="O6">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="P3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2033,77 +2244,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2116,7 +2334,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2128,96 +2346,96 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="F1" s="4"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="1"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -2262,432 +2480,436 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M20"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="A1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E4" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="A9" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>205</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="A13" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="A17" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>222</v>
-      </c>
       <c r="H18" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="L18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="M18" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="J19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>240</v>
-      </c>
       <c r="I20" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>2</v>
@@ -2721,25 +2943,25 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2747,54 +2969,54 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E6" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E7" s="10" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2811,25 +3033,28 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2860,53 +3085,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="A1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -2914,83 +3139,83 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="A5" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -3025,82 +3250,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>277</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3113,41 +3338,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3159,9 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3169,98 +3395,123 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3284,145 +3535,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C5" s="17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" s="21" t="s">
+    </row>
+    <row r="13" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="C6" s="21" t="s">
+    <row r="15" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="C7" s="21"/>
-    </row>
-    <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3432,10 +3683,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3446,76 +3697,122 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
         <v>53</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3524,131 +3821,212 @@
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" customWidth="1"/>
+    <col min="7" max="7" width="22.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.08984375" customWidth="1"/>
     <col min="12" max="12" width="9.1796875" customWidth="1"/>
     <col min="13" max="13" width="9.26953125" customWidth="1"/>
-    <col min="14" max="14" width="5.90625" customWidth="1"/>
+    <col min="14" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="14" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="E1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="21" t="s">
+      <c r="D2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1234567890</v>
+      </c>
+      <c r="H2" s="17">
+        <v>1234741258</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="21">
-        <v>1234567890</v>
-      </c>
-      <c r="H2" s="21">
-        <v>1234741258</v>
-      </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="17">
+        <v>12345</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="21">
-        <v>55555</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+    </row>
+    <row r="3" spans="1:15" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="G3" s="17">
+        <v>123456789</v>
+      </c>
+      <c r="H3" s="17">
+        <v>123456789</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17">
+        <v>1234</v>
+      </c>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="24"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="27">
+        <v>1234567890123</v>
+      </c>
+      <c r="H4" s="27">
+        <v>1234567890123</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="27">
+        <v>1234567</v>
+      </c>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="O6" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3668,76 +4046,76 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -3764,162 +4142,162 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>337</v>
+        <v>331</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>332</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="O2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="Q2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="Q3" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -3936,7 +4314,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -3985,55 +4363,55 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -4059,68 +4437,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="C4" s="25"/>
+        <v>335</v>
+      </c>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
@@ -4136,7 +4514,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4149,16 +4527,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4169,7 +4547,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -4181,16 +4559,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4200,19 +4578,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -4221,19 +4599,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -4243,16 +4621,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -4262,16 +4640,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -4290,12 +4668,12 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4304,16 +4682,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -4324,7 +4702,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -4336,16 +4714,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -4355,19 +4733,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -4376,19 +4754,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -4398,16 +4776,16 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -4416,16 +4794,16 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -4433,43 +4811,43 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="4"/>
     </row>
@@ -4487,10 +4865,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4501,71 +4879,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4573,7 +4951,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4581,87 +4959,87 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>375</v>
-      </c>
-      <c r="B13" s="24">
-        <v>8</v>
+        <v>370</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B15">
-        <v>251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B17">
-        <v>1700000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B18">
-        <v>100650</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B19">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B20">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B21">
         <v>7</v>
@@ -4669,7 +5047,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -4677,7 +5055,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4685,9 +5063,25 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change-Id: I0000000000000000000000000000000000000000 Rajeev's Changes till 08 Nov 2021
Change-Id: I6970f79cdb7afcdc591578d9d6459ee246a1c138
</commit_message>
<xml_diff>
--- a/BITSAUTOMATION/excel/TestData.xlsx
+++ b/BITSAUTOMATION/excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" tabRatio="924" firstSheet="9" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050" tabRatio="924" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="388">
   <si>
     <t>username</t>
   </si>
@@ -533,15 +533,9 @@
     <t>Edited Project Desc</t>
   </si>
   <si>
-    <t>Onida-Chennai</t>
-  </si>
-  <si>
     <t>Sem1</t>
   </si>
   <si>
-    <t>New Project</t>
-  </si>
-  <si>
     <t>Project Description</t>
   </si>
   <si>
@@ -1199,13 +1193,16 @@
     <t>Viram Technologies</t>
   </si>
   <si>
-    <t>2021-21</t>
-  </si>
-  <si>
     <t>2022-23</t>
   </si>
   <si>
     <t>2023-24</t>
+  </si>
+  <si>
+    <t>ABC Info</t>
+  </si>
+  <si>
+    <t>New Project Test</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1391,6 +1388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1706,39 +1704,39 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
@@ -1756,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
@@ -1770,13 +1768,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
@@ -1790,13 +1788,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
@@ -1810,13 +1808,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
@@ -1830,13 +1828,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
@@ -2087,10 +2085,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>133</v>
@@ -2138,10 +2136,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>123</v>
@@ -2219,7 +2217,7 @@
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L6">
         <v>11</v>
@@ -2477,14 +2475,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2544,58 +2544,58 @@
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>78</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="K4" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -2608,13 +2608,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>180</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>76</v>
@@ -2623,50 +2623,50 @@
         <v>4</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -2679,72 +2679,72 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>192</v>
       </c>
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -2757,31 +2757,31 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -2794,25 +2794,25 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>215</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>119</v>
@@ -2835,31 +2835,31 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>13</v>
@@ -2871,36 +2871,36 @@
         <v>15</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>235</v>
-      </c>
       <c r="I20" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>13</v>
@@ -2913,6 +2913,11 @@
       </c>
       <c r="M20" s="4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J21" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -2949,19 +2954,19 @@
         <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2989,7 +2994,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>12</v>
@@ -3003,7 +3008,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>152</v>
@@ -3011,12 +3016,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E6" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E7" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3044,7 +3049,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -3086,7 +3091,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3107,31 +3112,31 @@
         <v>102</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>70</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>250</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3145,27 +3150,27 @@
         <v>79</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -3200,10 +3205,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -3215,7 +3220,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3250,82 +3255,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>264</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3430,7 +3435,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>12</v>
@@ -3439,7 +3444,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>39</v>
@@ -3474,7 +3479,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -3487,7 +3492,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>32</v>
@@ -3536,96 +3541,96 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -3636,10 +3641,10 @@
     <row r="12" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3647,33 +3652,33 @@
         <v>5</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -3685,8 +3690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3723,7 +3728,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -3765,9 +3770,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>153</v>
@@ -3778,7 +3791,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>386</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -3792,13 +3805,13 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3895,7 +3908,7 @@
         <v>28</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G2" s="17">
         <v>1234567890</v>
@@ -3936,7 +3949,7 @@
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G3" s="17">
         <v>123456789</v>
@@ -3947,7 +3960,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -3987,10 +4000,10 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -3998,7 +4011,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O5" s="3"/>
     </row>
@@ -4017,7 +4030,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="17" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="O6" s="3"/>
     </row>
@@ -4067,10 +4080,10 @@
         <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4087,7 +4100,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -4115,7 +4128,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -4193,15 +4206,15 @@
         <v>17</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>76</v>
@@ -4213,10 +4226,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>78</v>
@@ -4249,7 +4262,7 @@
         <v>84</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -4297,7 +4310,7 @@
         <v>92</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -4314,7 +4327,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -4384,7 +4397,7 @@
         <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -4396,7 +4409,7 @@
         <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -4458,10 +4471,10 @@
         <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4469,7 +4482,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C4" s="21"/>
     </row>
@@ -4478,14 +4491,14 @@
         <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -4547,7 +4560,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -4562,7 +4575,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>48</v>
@@ -4602,7 +4615,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>40</v>
@@ -4811,10 +4824,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -4841,7 +4854,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B23" s="4"/>
     </row>
@@ -4879,18 +4892,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -4898,20 +4911,20 @@
         <v>151</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4919,7 +4932,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4927,7 +4940,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4935,7 +4948,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4943,7 +4956,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4951,7 +4964,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4959,7 +4972,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4967,7 +4980,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4975,7 +4988,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B13" s="20">
         <v>0</v>
@@ -4983,7 +4996,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4991,7 +5004,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4999,7 +5012,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5007,7 +5020,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5015,7 +5028,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5023,7 +5036,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5031,7 +5044,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -5039,7 +5052,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B21">
         <v>7</v>
@@ -5063,7 +5076,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5071,7 +5084,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5079,7 +5092,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B26">
         <v>0</v>

</xml_diff>